<commit_message>
Atualizando plano de ação sprint 2c
</commit_message>
<xml_diff>
--- a/sprint_grupo7/TI/Modelo-Plano-De-Acao.xlsx
+++ b/sprint_grupo7/TI/Modelo-Plano-De-Acao.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amand\Documents\SPRINT\sprint_02\sprint_grupo7\TI\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E3FB035-A131-49A5-B913-C0E017A855C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10305" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Plano de Ação" sheetId="1" r:id="rId1"/>
@@ -22,16 +16,16 @@
     <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
+    <definedName name="Interval" localSheetId="1">'[1]Return to Work Template'!#REF!</definedName>
+    <definedName name="Interval">'[1]Return to Work Template'!#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Plano de Ação'!$B$1:$H$28</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Plano de Ação - EM BRANCO'!$B$1:$H$28</definedName>
-    <definedName name="Interval" localSheetId="1">'[1]Return to Work Template'!#REF!</definedName>
-    <definedName name="Interval">'[1]Return to Work Template'!#REF!</definedName>
     <definedName name="ScheduleStart" localSheetId="1">'[1]Return to Work Template'!#REF!</definedName>
     <definedName name="ScheduleStart">'[1]Return to Work Template'!#REF!</definedName>
     <definedName name="Type" localSheetId="1">'[2]Maintenance Work Order'!#REF!</definedName>
     <definedName name="Type">'[2]Maintenance Work Order'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -49,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="72">
   <si>
     <t>MODELO DE PLANO DE AÇÃO</t>
   </si>
@@ -90,9 +84,6 @@
     <t>Em andamento</t>
   </si>
   <si>
-    <t>CLIQUE AQUI PARA CRIAR NO SMARTSHEET</t>
-  </si>
-  <si>
     <t>PLANO DE AÇÃO</t>
   </si>
   <si>
@@ -196,17 +187,89 @@
   </si>
   <si>
     <t>Eduardo/Igor/Amanda</t>
+  </si>
+  <si>
+    <t>Tela inicial</t>
+  </si>
+  <si>
+    <t>Fernanda/Cauê</t>
+  </si>
+  <si>
+    <t>Footer</t>
+  </si>
+  <si>
+    <t>Eduardo</t>
+  </si>
+  <si>
+    <t>Tela suporte</t>
+  </si>
+  <si>
+    <t>Tela recurso</t>
+  </si>
+  <si>
+    <t>Fernanda</t>
+  </si>
+  <si>
+    <t>Igor</t>
+  </si>
+  <si>
+    <t>Tela plataforma</t>
+  </si>
+  <si>
+    <t>Cauê</t>
+  </si>
+  <si>
+    <t>2023-10-16</t>
+  </si>
+  <si>
+    <t>Tela perfil</t>
+  </si>
+  <si>
+    <t>Gráfico de burndown</t>
+  </si>
+  <si>
+    <t>2023-10-20</t>
+  </si>
+  <si>
+    <t>Complero</t>
+  </si>
+  <si>
+    <t>Atualização do product backlog</t>
+  </si>
+  <si>
+    <t>Inclusão das prioridades e seus tamanhos</t>
+  </si>
+  <si>
+    <t>Objetivo 2c: Finalização das telas</t>
+  </si>
+  <si>
+    <t>Thiago/Cauê</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sobre nós </t>
+  </si>
+  <si>
+    <t>Tela login</t>
+  </si>
+  <si>
+    <t>Amanda/Giovanna</t>
+  </si>
+  <si>
+    <t>Tela cadastro</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -277,19 +340,6 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="22"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="0"/>
       <name val="Century Gothic"/>
@@ -302,7 +352,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -331,12 +381,6 @@
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00BD32"/>
-        <bgColor rgb="FF00BD32"/>
       </patternFill>
     </fill>
   </fills>
@@ -373,12 +417,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -438,23 +481,22 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="5">
-    <cellStyle name="Hiperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="4" builtinId="8"/>
-    <cellStyle name="Hiperlink Visitado" xfId="2" builtinId="9" hidden="1"/>
+  <cellStyles count="4">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 2" xfId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -470,7 +512,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Return to Work Template"/>
@@ -483,7 +525,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Maintenance Work Order"/>
@@ -820,28 +862,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q30"/>
+  <dimension ref="A1:Q38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" customWidth="1"/>
-    <col min="2" max="2" width="31.83203125" customWidth="1"/>
+    <col min="1" max="1" width="3.375" customWidth="1"/>
+    <col min="2" max="2" width="31.875" customWidth="1"/>
     <col min="3" max="3" width="19.5" customWidth="1"/>
-    <col min="4" max="5" width="15.6640625" customWidth="1"/>
-    <col min="6" max="6" width="13.4140625" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" customWidth="1"/>
+    <col min="4" max="5" width="15.625" customWidth="1"/>
+    <col min="6" max="6" width="13.375" customWidth="1"/>
+    <col min="7" max="7" width="12.375" customWidth="1"/>
     <col min="8" max="8" width="40" customWidth="1"/>
-    <col min="9" max="9" width="3.33203125" customWidth="1"/>
+    <col min="9" max="9" width="3.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="45" customHeight="1">
@@ -851,7 +893,7 @@
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:17" s="6" customFormat="1" ht="22.25" customHeight="1">
+    <row r="2" spans="1:17" s="6" customFormat="1" ht="22.35" customHeight="1">
       <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
@@ -873,12 +915,12 @@
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
     </row>
-    <row r="3" spans="1:17" s="6" customFormat="1" ht="22.25" customHeight="1">
+    <row r="3" spans="1:17" s="6" customFormat="1" ht="22.35" customHeight="1">
       <c r="B3" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>27</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>28</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
@@ -895,7 +937,7 @@
       <c r="P3" s="8"/>
       <c r="Q3" s="8"/>
     </row>
-    <row r="4" spans="1:17" ht="11" customHeight="1">
+    <row r="4" spans="1:17" ht="11.1" customHeight="1">
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -904,7 +946,7 @@
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:17" ht="20" customHeight="1">
+    <row r="5" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="B5" s="10" t="s">
         <v>3</v>
       </c>
@@ -927,9 +969,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="20" customHeight="1">
+    <row r="6" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="B6" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -938,18 +980,18 @@
       <c r="G6" s="14"/>
       <c r="H6" s="17"/>
     </row>
-    <row r="7" spans="1:17" ht="20" customHeight="1">
+    <row r="7" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="B7" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="11" t="s">
         <v>20</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>21</v>
       </c>
       <c r="F7" s="19">
         <v>45194</v>
@@ -959,18 +1001,18 @@
       </c>
       <c r="H7" s="18"/>
     </row>
-    <row r="8" spans="1:17" ht="19.75" customHeight="1">
+    <row r="8" spans="1:17" ht="19.7" customHeight="1">
       <c r="B8" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F8" s="19">
         <v>45194</v>
@@ -980,18 +1022,18 @@
       </c>
       <c r="H8" s="18"/>
     </row>
-    <row r="9" spans="1:17" ht="28.25" customHeight="1">
+    <row r="9" spans="1:17" ht="28.35" customHeight="1">
       <c r="B9" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>47</v>
+        <v>25</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>46</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F9" s="19">
         <v>45194</v>
@@ -1000,21 +1042,21 @@
         <v>45197</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="31.75" customHeight="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="31.7" customHeight="1">
       <c r="B10" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="11" t="s">
         <v>20</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>21</v>
       </c>
       <c r="F10" s="19">
         <v>45194</v>
@@ -1024,18 +1066,18 @@
       </c>
       <c r="H10" s="18"/>
     </row>
-    <row r="11" spans="1:17" ht="20" customHeight="1">
+    <row r="11" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="B11" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F11" s="19">
         <v>45194</v>
@@ -1045,18 +1087,18 @@
       </c>
       <c r="H11" s="21"/>
     </row>
-    <row r="12" spans="1:17" ht="20" customHeight="1">
+    <row r="12" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="B12" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="11" t="s">
-        <v>25</v>
-      </c>
       <c r="D12" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F12" s="19">
         <v>45194</v>
@@ -1065,10 +1107,10 @@
         <v>45197</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" ht="20" customHeight="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="B13" s="18"/>
       <c r="C13" s="20"/>
       <c r="D13" s="11"/>
@@ -1077,7 +1119,7 @@
       <c r="G13" s="19"/>
       <c r="H13" s="18"/>
     </row>
-    <row r="14" spans="1:17" ht="20" customHeight="1">
+    <row r="14" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="B14" s="10" t="s">
         <v>3</v>
       </c>
@@ -1100,9 +1142,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="20" customHeight="1">
+    <row r="15" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="B15" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
@@ -1111,18 +1153,18 @@
       <c r="G15" s="16"/>
       <c r="H15" s="17"/>
     </row>
-    <row r="16" spans="1:17" ht="20" customHeight="1">
+    <row r="16" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="B16" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D16" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F16" s="19">
         <v>45199</v>
@@ -1131,21 +1173,21 @@
         <v>45204</v>
       </c>
       <c r="H16" s="18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" ht="20" customHeight="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B17" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D17" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F17" s="19">
         <v>45200</v>
@@ -1154,21 +1196,21 @@
         <v>45204</v>
       </c>
       <c r="H17" s="18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" ht="20" customHeight="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B18" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D18" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F18" s="19">
         <v>45200</v>
@@ -1177,15 +1219,15 @@
         <v>45204</v>
       </c>
       <c r="H18" s="18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" ht="20" customHeight="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B19" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D19" s="11" t="s">
         <v>10</v>
@@ -1200,21 +1242,21 @@
         <v>45204</v>
       </c>
       <c r="H19" s="18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" ht="20" customHeight="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B20" s="18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D20" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F20" s="19">
         <v>45200</v>
@@ -1223,15 +1265,15 @@
         <v>45204</v>
       </c>
       <c r="H20" s="18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" ht="20" customHeight="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B21" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D21" s="11" t="s">
         <v>10</v>
@@ -1246,10 +1288,10 @@
         <v>45204</v>
       </c>
       <c r="H21" s="18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" ht="20" customHeight="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B22" s="18"/>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
@@ -1258,85 +1300,322 @@
       <c r="G22" s="12"/>
       <c r="H22" s="18"/>
     </row>
-    <row r="23" spans="2:8" ht="20" customHeight="1">
-      <c r="B23" s="17"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="17"/>
-    </row>
-    <row r="24" spans="2:8" ht="20" customHeight="1">
-      <c r="B24" s="18"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="18"/>
-    </row>
-    <row r="25" spans="2:8" ht="20" customHeight="1">
-      <c r="B25" s="18"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
+    <row r="23" spans="2:8" ht="20.100000000000001" customHeight="1">
+      <c r="B23" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="20.100000000000001" customHeight="1">
+      <c r="B24" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="17"/>
+    </row>
+    <row r="25" spans="2:8" ht="20.100000000000001" customHeight="1">
+      <c r="B25" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="19">
+        <v>45215</v>
+      </c>
+      <c r="G25" s="19">
+        <v>45219</v>
+      </c>
       <c r="H25" s="18"/>
     </row>
-    <row r="26" spans="2:8" ht="20" customHeight="1">
-      <c r="B26" s="18"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
+    <row r="26" spans="2:8" ht="20.100000000000001" customHeight="1">
+      <c r="B26" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="19">
+        <v>45215</v>
+      </c>
+      <c r="G26" s="19">
+        <v>45219</v>
+      </c>
       <c r="H26" s="18"/>
     </row>
-    <row r="27" spans="2:8" ht="20" customHeight="1">
-      <c r="B27" s="18"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
+    <row r="27" spans="2:8" ht="20.100000000000001" customHeight="1">
+      <c r="B27" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" s="19">
+        <v>45215</v>
+      </c>
+      <c r="G27" s="19">
+        <v>45219</v>
+      </c>
       <c r="H27" s="18"/>
     </row>
-    <row r="28" spans="2:8" ht="20" customHeight="1">
-      <c r="B28" s="18"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
+    <row r="28" spans="2:8" ht="19.5" customHeight="1">
+      <c r="B28" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G28" s="23" t="s">
+        <v>61</v>
+      </c>
       <c r="H28" s="18"/>
     </row>
-    <row r="30" spans="2:8" s="1" customFormat="1" ht="50" customHeight="1">
-      <c r="B30" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" s="23"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="23"/>
+    <row r="29" spans="2:8" ht="19.5" customHeight="1">
+      <c r="B29" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F29" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G29" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="H29" s="18"/>
+    </row>
+    <row r="30" spans="2:8" ht="19.5" customHeight="1">
+      <c r="B30" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G30" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="H30" s="18"/>
+    </row>
+    <row r="31" spans="2:8" ht="19.5" customHeight="1">
+      <c r="B31" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F31" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G31" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="H31" s="18"/>
+    </row>
+    <row r="32" spans="2:8" ht="28.5" customHeight="1">
+      <c r="B32" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F32" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="G32" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="H32" s="18"/>
+    </row>
+    <row r="33" spans="2:8" ht="27">
+      <c r="B33" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F33" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="G33" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="H33" s="18"/>
+    </row>
+    <row r="34" spans="2:8" ht="19.5" customHeight="1">
+      <c r="B34" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F34" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G34" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="H34" s="18"/>
+    </row>
+    <row r="35" spans="2:8" ht="19.5" customHeight="1">
+      <c r="B35" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F35" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G35" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="H35" s="18"/>
+    </row>
+    <row r="36" spans="2:8">
+      <c r="B36" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F36" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G36" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="H36" s="18"/>
+    </row>
+    <row r="37" spans="2:8" ht="19.5" customHeight="1">
+      <c r="B37" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F37" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G37" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="H37" s="18"/>
+    </row>
+    <row r="38" spans="2:8" ht="19.5" customHeight="1">
+      <c r="G38" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B30:H30"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="B30" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-  </hyperlinks>
   <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0" footer="0"/>
-  <pageSetup scale="83" fitToHeight="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId2"/>
+  <pageSetup scale="83" fitToHeight="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
     <pageSetUpPr fitToPage="1"/>
@@ -1347,26 +1626,26 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" customWidth="1"/>
-    <col min="2" max="2" width="31.83203125" customWidth="1"/>
+    <col min="1" max="1" width="3.375" customWidth="1"/>
+    <col min="2" max="2" width="31.875" customWidth="1"/>
     <col min="3" max="3" width="19.5" customWidth="1"/>
-    <col min="4" max="5" width="15.6640625" customWidth="1"/>
-    <col min="6" max="6" width="13.4140625" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" customWidth="1"/>
+    <col min="4" max="5" width="15.625" customWidth="1"/>
+    <col min="6" max="6" width="13.375" customWidth="1"/>
+    <col min="7" max="7" width="12.375" customWidth="1"/>
     <col min="8" max="8" width="40" customWidth="1"/>
-    <col min="9" max="9" width="3.33203125" customWidth="1"/>
+    <col min="9" max="9" width="3.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="45" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:17" s="6" customFormat="1" ht="22.25" customHeight="1">
+    <row r="2" spans="1:17" s="6" customFormat="1" ht="22.35" customHeight="1">
       <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
@@ -1388,7 +1667,7 @@
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
     </row>
-    <row r="3" spans="1:17" s="6" customFormat="1" ht="22.25" customHeight="1">
+    <row r="3" spans="1:17" s="6" customFormat="1" ht="22.35" customHeight="1">
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
       <c r="D3" s="8"/>
@@ -1406,7 +1685,7 @@
       <c r="P3" s="8"/>
       <c r="Q3" s="8"/>
     </row>
-    <row r="4" spans="1:17" ht="11" customHeight="1">
+    <row r="4" spans="1:17" ht="11.1" customHeight="1">
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -1415,7 +1694,7 @@
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:17" ht="20" customHeight="1">
+    <row r="5" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="B5" s="10" t="s">
         <v>3</v>
       </c>
@@ -1438,9 +1717,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="20" customHeight="1">
+    <row r="6" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="B6" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -1449,7 +1728,7 @@
       <c r="G6" s="14"/>
       <c r="H6" s="17"/>
     </row>
-    <row r="7" spans="1:17" ht="20" customHeight="1">
+    <row r="7" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="B7" s="18"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
@@ -1458,7 +1737,7 @@
       <c r="G7" s="12"/>
       <c r="H7" s="18"/>
     </row>
-    <row r="8" spans="1:17" ht="20" customHeight="1">
+    <row r="8" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="B8" s="18"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
@@ -1467,7 +1746,7 @@
       <c r="G8" s="12"/>
       <c r="H8" s="18"/>
     </row>
-    <row r="9" spans="1:17" ht="20" customHeight="1">
+    <row r="9" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="B9" s="18"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
@@ -1476,7 +1755,7 @@
       <c r="G9" s="12"/>
       <c r="H9" s="18"/>
     </row>
-    <row r="10" spans="1:17" ht="20" customHeight="1">
+    <row r="10" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="B10" s="18"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
@@ -1485,9 +1764,9 @@
       <c r="G10" s="12"/>
       <c r="H10" s="18"/>
     </row>
-    <row r="11" spans="1:17" ht="20" customHeight="1">
+    <row r="11" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="B11" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
@@ -1496,7 +1775,7 @@
       <c r="G11" s="16"/>
       <c r="H11" s="17"/>
     </row>
-    <row r="12" spans="1:17" ht="20" customHeight="1">
+    <row r="12" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="B12" s="18"/>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
@@ -1505,7 +1784,7 @@
       <c r="G12" s="12"/>
       <c r="H12" s="18"/>
     </row>
-    <row r="13" spans="1:17" ht="20" customHeight="1">
+    <row r="13" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="B13" s="18"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
@@ -1514,7 +1793,7 @@
       <c r="G13" s="12"/>
       <c r="H13" s="18"/>
     </row>
-    <row r="14" spans="1:17" ht="20" customHeight="1">
+    <row r="14" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="B14" s="18"/>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
@@ -1523,7 +1802,7 @@
       <c r="G14" s="12"/>
       <c r="H14" s="18"/>
     </row>
-    <row r="15" spans="1:17" ht="20" customHeight="1">
+    <row r="15" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="B15" s="18"/>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
@@ -1532,7 +1811,7 @@
       <c r="G15" s="12"/>
       <c r="H15" s="18"/>
     </row>
-    <row r="16" spans="1:17" ht="20" customHeight="1">
+    <row r="16" spans="1:17" ht="20.100000000000001" customHeight="1">
       <c r="B16" s="18"/>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
@@ -1541,9 +1820,9 @@
       <c r="G16" s="12"/>
       <c r="H16" s="18"/>
     </row>
-    <row r="17" spans="2:8" ht="20" customHeight="1">
+    <row r="17" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B17" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
@@ -1552,7 +1831,7 @@
       <c r="G17" s="16"/>
       <c r="H17" s="17"/>
     </row>
-    <row r="18" spans="2:8" ht="20" customHeight="1">
+    <row r="18" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B18" s="18"/>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
@@ -1561,7 +1840,7 @@
       <c r="G18" s="12"/>
       <c r="H18" s="18"/>
     </row>
-    <row r="19" spans="2:8" ht="20" customHeight="1">
+    <row r="19" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B19" s="18"/>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
@@ -1570,7 +1849,7 @@
       <c r="G19" s="12"/>
       <c r="H19" s="18"/>
     </row>
-    <row r="20" spans="2:8" ht="20" customHeight="1">
+    <row r="20" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B20" s="18"/>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
@@ -1579,7 +1858,7 @@
       <c r="G20" s="12"/>
       <c r="H20" s="18"/>
     </row>
-    <row r="21" spans="2:8" ht="20" customHeight="1">
+    <row r="21" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B21" s="18"/>
       <c r="C21" s="11"/>
       <c r="D21" s="11"/>
@@ -1588,7 +1867,7 @@
       <c r="G21" s="12"/>
       <c r="H21" s="18"/>
     </row>
-    <row r="22" spans="2:8" ht="20" customHeight="1">
+    <row r="22" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B22" s="18"/>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
@@ -1597,9 +1876,9 @@
       <c r="G22" s="12"/>
       <c r="H22" s="18"/>
     </row>
-    <row r="23" spans="2:8" ht="20" customHeight="1">
+    <row r="23" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B23" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
@@ -1608,7 +1887,7 @@
       <c r="G23" s="16"/>
       <c r="H23" s="17"/>
     </row>
-    <row r="24" spans="2:8" ht="20" customHeight="1">
+    <row r="24" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B24" s="18"/>
       <c r="C24" s="11"/>
       <c r="D24" s="11"/>
@@ -1617,7 +1896,7 @@
       <c r="G24" s="12"/>
       <c r="H24" s="18"/>
     </row>
-    <row r="25" spans="2:8" ht="20" customHeight="1">
+    <row r="25" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B25" s="18"/>
       <c r="C25" s="11"/>
       <c r="D25" s="11"/>
@@ -1626,7 +1905,7 @@
       <c r="G25" s="12"/>
       <c r="H25" s="18"/>
     </row>
-    <row r="26" spans="2:8" ht="20" customHeight="1">
+    <row r="26" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B26" s="18"/>
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
@@ -1635,7 +1914,7 @@
       <c r="G26" s="12"/>
       <c r="H26" s="18"/>
     </row>
-    <row r="27" spans="2:8" ht="20" customHeight="1">
+    <row r="27" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B27" s="18"/>
       <c r="C27" s="11"/>
       <c r="D27" s="11"/>
@@ -1644,7 +1923,7 @@
       <c r="G27" s="12"/>
       <c r="H27" s="18"/>
     </row>
-    <row r="28" spans="2:8" ht="20" customHeight="1">
+    <row r="28" spans="2:8" ht="20.100000000000001" customHeight="1">
       <c r="B28" s="18"/>
       <c r="C28" s="13"/>
       <c r="D28" s="13"/>
@@ -1660,7 +1939,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
@@ -1670,18 +1949,18 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="88.33203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="3"/>
+    <col min="1" max="1" width="3.375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="88.375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.875" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="10.875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="20" customHeight="1"/>
+    <row r="1" spans="2:2" ht="20.100000000000001" customHeight="1"/>
     <row r="2" spans="2:2" ht="105" customHeight="1">
       <c r="B2" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Inserindo tela plataforma no site
</commit_message>
<xml_diff>
--- a/sprint_grupo7/TI/Modelo-Plano-De-Acao.xlsx
+++ b/sprint_grupo7/TI/Modelo-Plano-De-Acao.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\SP-TECH\Pesquisa e inovação (PI)\Trabalho tomates\Plantação de tomate\sprint_02\sprint_grupo7\TI\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C8733F-3008-410D-8129-8D964196CB93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10305" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13290" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plano de Ação" sheetId="1" r:id="rId1"/>
@@ -16,34 +22,21 @@
     <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Plano de Ação'!$B$1:$H$28</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Plano de Ação - EM BRANCO'!$B$1:$H$28</definedName>
     <definedName name="Interval" localSheetId="1">'[1]Return to Work Template'!#REF!</definedName>
     <definedName name="Interval">'[1]Return to Work Template'!#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Plano de Ação'!$B$1:$H$28</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Plano de Ação - EM BRANCO'!$B$1:$H$28</definedName>
     <definedName name="ScheduleStart" localSheetId="1">'[1]Return to Work Template'!#REF!</definedName>
     <definedName name="ScheduleStart">'[1]Return to Work Template'!#REF!</definedName>
     <definedName name="Type" localSheetId="1">'[2]Maintenance Work Order'!#REF!</definedName>
     <definedName name="Type">'[2]Maintenance Work Order'!#REF!</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="75">
   <si>
     <t>MODELO DE PLANO DE AÇÃO</t>
   </si>
@@ -259,17 +252,26 @@
   </si>
   <si>
     <t>Dashboard</t>
+  </si>
+  <si>
+    <t>Iniciação da tela de login e suas validações.</t>
+  </si>
+  <si>
+    <t>Iniciação da tela de cadastro e suas validações.</t>
+  </si>
+  <si>
+    <t>Alterações finais na estilização e alertas.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="14">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -351,6 +353,21 @@
       <name val="Century Gothic"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Century Gothic"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -423,7 +440,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -491,12 +508,19 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperlink Visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -512,7 +536,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Return to Work Template"/>
@@ -525,7 +549,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Maintenance Work Order"/>
@@ -862,7 +886,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
@@ -870,8 +894,8 @@
   <dimension ref="A1:Q38"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -892,6 +916,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="2"/>
+      <c r="E1" s="26"/>
     </row>
     <row r="2" spans="1:17" s="6" customFormat="1" ht="22.35" customHeight="1">
       <c r="B2" s="7" t="s">
@@ -1153,7 +1178,7 @@
       <c r="G15" s="16"/>
       <c r="H15" s="17"/>
     </row>
-    <row r="16" spans="1:17" ht="20.100000000000001" customHeight="1">
+    <row r="16" spans="1:17" ht="33" customHeight="1">
       <c r="B16" s="18" t="s">
         <v>35</v>
       </c>
@@ -1164,7 +1189,7 @@
         <v>10</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F16" s="19">
         <v>45199</v>
@@ -1173,7 +1198,7 @@
         <v>45204</v>
       </c>
       <c r="H16" s="18" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="20.100000000000001" customHeight="1">
@@ -1187,7 +1212,7 @@
         <v>10</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F17" s="19">
         <v>45200</v>
@@ -1196,7 +1221,7 @@
         <v>45204</v>
       </c>
       <c r="H17" s="18" t="s">
-        <v>44</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="20.100000000000001" customHeight="1">
@@ -1210,7 +1235,7 @@
         <v>10</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F18" s="19">
         <v>45200</v>
@@ -1278,7 +1303,7 @@
       <c r="D21" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E21" s="25" t="s">
         <v>11</v>
       </c>
       <c r="F21" s="19">
@@ -1347,7 +1372,7 @@
       <c r="E25" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F25" s="19">
+      <c r="F25" s="27">
         <v>45215</v>
       </c>
       <c r="G25" s="19">
@@ -1563,7 +1588,9 @@
       <c r="G35" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="H35" s="18"/>
+      <c r="H35" s="18" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="36" spans="2:8">
       <c r="B36" s="18" t="s">
@@ -1584,7 +1611,9 @@
       <c r="G36" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="H36" s="18"/>
+      <c r="H36" s="18" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="37" spans="2:8" ht="19.5" customHeight="1">
       <c r="B37" s="18" t="s">
@@ -1615,7 +1644,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
     <pageSetUpPr fitToPage="1"/>
@@ -1939,7 +1968,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>

</xml_diff>